<commit_message>
Add new module. DoronG
</commit_message>
<xml_diff>
--- a/dorong.xlsx
+++ b/dorong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StockExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60C02C98-635A-474A-99A3-86FEE5C28A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{107B85C6-54B0-4A23-9DD4-D99B325B5BCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{9FBD4CBC-5FD8-4A40-904A-9428D68F7053}"/>
+    <workbookView xWindow="32310" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{A734250A-07F2-4A15-A70F-AB0A6A3A0105}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9DCE37-C0E1-4034-B02C-35F411C16162}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB4C0CB-9E87-4436-8AA3-55FE738ABE1E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>